<commit_message>
[MS-MEETS]: Add and update cases and capture code for latest RS
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-MEETS/MS-MEETS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-MEETS/MS-MEETS_RequirementSpecification.xlsx
@@ -11371,13 +11371,13 @@
         <v>19</v>
       </c>
       <c r="F210" s="41" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G210" s="41" t="s">
         <v>15</v>
       </c>
       <c r="H210" s="41" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I210" s="42"/>
     </row>
@@ -15652,7 +15652,7 @@
         <v>15</v>
       </c>
       <c r="H381" s="41" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I381" s="42"/>
     </row>
@@ -19873,6 +19873,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -19921,37 +19936,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -19965,10 +19950,25 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>